<commit_message>
Gon try and break everything
Found a bug that causes the entry to be changed to NULL when you try to cancel renaming something. Working on fixing it.
</commit_message>
<xml_diff>
--- a/Excels/Test_Data.xlsx
+++ b/Excels/Test_Data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Bat Data\Bat Data\BatData\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryley\Desktop\Oakleigh Project\BatData\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3400BFB-5948-441C-8CF3-516B866C5B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F7CAD5-2FB7-4E75-93EE-2392BAC1ED23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Expected_Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Expected" sheetId="4" r:id="rId2"/>
+    <sheet name="asd" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="115">
   <si>
     <t>INDIR</t>
   </si>
@@ -368,6 +369,9 @@
   </si>
   <si>
     <t>Trawling</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -408,12 +412,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -428,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -439,6 +449,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="47" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P8" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -834,7 +852,7 @@
         <v>26</v>
       </c>
       <c r="D2">
-        <v>2023</v>
+        <v>200</v>
       </c>
       <c r="E2">
         <v>2.4607190000000001</v>
@@ -843,22 +861,22 @@
         <v>1.0835900000000001</v>
       </c>
       <c r="G2">
-        <v>38402.031000000003</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>39067.718999999997</v>
+        <v>50</v>
       </c>
       <c r="I2">
-        <v>40086.440999999999</v>
+        <v>100</v>
       </c>
       <c r="J2" s="1">
         <v>45006</v>
       </c>
       <c r="K2" s="2">
-        <v>0.77321134259259272</v>
+        <v>0.77320601851851856</v>
       </c>
       <c r="L2">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="M2" s="1">
         <v>45006</v>
@@ -908,7 +926,7 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <v>2023</v>
+        <v>201</v>
       </c>
       <c r="E3">
         <v>0.11068699999999999</v>
@@ -917,13 +935,13 @@
         <v>5.0884499999999999</v>
       </c>
       <c r="G3">
-        <v>38846.019999999997</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>40458.718999999997</v>
+        <v>51</v>
       </c>
       <c r="I3">
-        <v>46313.745999999999</v>
+        <v>101</v>
       </c>
       <c r="J3" s="1">
         <v>45006</v>
@@ -932,7 +950,7 @@
         <v>0.76921422453703703</v>
       </c>
       <c r="L3">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="M3" s="1">
         <v>45006</v>
@@ -982,7 +1000,7 @@
         <v>32</v>
       </c>
       <c r="D4">
-        <v>2023</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>5.7399999999999997E-4</v>
@@ -991,13 +1009,13 @@
         <v>4.8860380000000001</v>
       </c>
       <c r="G4">
-        <v>38654.038999999997</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>39736.027000000002</v>
+        <v>52</v>
       </c>
       <c r="I4">
-        <v>42603.258000000002</v>
+        <v>102</v>
       </c>
       <c r="J4" s="1">
         <v>45006</v>
@@ -1006,7 +1024,7 @@
         <v>0.7722106481481481</v>
       </c>
       <c r="L4">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M4" s="1">
         <v>45006</v>
@@ -1053,7 +1071,7 @@
         <v>101</v>
       </c>
       <c r="D5">
-        <v>2024</v>
+        <v>203</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1062,13 +1080,13 @@
         <v>4</v>
       </c>
       <c r="G5">
-        <v>43204.55</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>40000.050000000003</v>
+        <v>53</v>
       </c>
       <c r="I5">
-        <v>42666.25</v>
+        <v>103</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>100</v>
@@ -1077,7 +1095,7 @@
         <v>0.77784722222222225</v>
       </c>
       <c r="L5">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="M5" s="1">
         <v>45769</v>
@@ -1124,7 +1142,7 @@
         <v>34</v>
       </c>
       <c r="D6">
-        <v>2023</v>
+        <v>204</v>
       </c>
       <c r="E6">
         <v>0.105099</v>
@@ -1133,13 +1151,13 @@
         <v>4.0046530000000002</v>
       </c>
       <c r="G6">
-        <v>34144.305</v>
+        <v>5</v>
       </c>
       <c r="H6">
-        <v>35101.711000000003</v>
+        <v>54</v>
       </c>
       <c r="I6">
-        <v>37318.620999999999</v>
+        <v>104</v>
       </c>
       <c r="J6" s="1">
         <v>45006</v>
@@ -1148,7 +1166,7 @@
         <v>0.77328824074074076</v>
       </c>
       <c r="L6">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="M6" s="1">
         <v>45006</v>
@@ -1198,7 +1216,7 @@
         <v>37</v>
       </c>
       <c r="D7">
-        <v>2023</v>
+        <v>205</v>
       </c>
       <c r="E7">
         <v>0.20311799999999999</v>
@@ -1207,13 +1225,13 @@
         <v>2.536276</v>
       </c>
       <c r="G7">
-        <v>39698.879000000001</v>
+        <v>6</v>
       </c>
       <c r="H7">
-        <v>40574.574000000001</v>
+        <v>55</v>
       </c>
       <c r="I7">
-        <v>43022.491999999998</v>
+        <v>105</v>
       </c>
       <c r="J7" s="1">
         <v>45006</v>
@@ -1222,7 +1240,7 @@
         <v>0.77392594907407408</v>
       </c>
       <c r="L7">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="M7" s="1">
         <v>45006</v>
@@ -1272,7 +1290,7 @@
         <v>37</v>
       </c>
       <c r="D8">
-        <v>2023</v>
+        <v>206</v>
       </c>
       <c r="E8">
         <v>3.2811599999999999</v>
@@ -1281,13 +1299,13 @@
         <v>0.56670500000000001</v>
       </c>
       <c r="G8">
-        <v>38716.445</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>39157.836000000003</v>
+        <v>56</v>
       </c>
       <c r="I8">
-        <v>40274.858999999997</v>
+        <v>106</v>
       </c>
       <c r="J8" s="1">
         <v>45006</v>
@@ -1296,7 +1314,7 @@
         <v>0.77396157407407407</v>
       </c>
       <c r="L8">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="M8" s="1">
         <v>45006</v>
@@ -1346,7 +1364,7 @@
         <v>39</v>
       </c>
       <c r="D9">
-        <v>2023</v>
+        <v>207</v>
       </c>
       <c r="E9">
         <v>6.0800000000000003E-4</v>
@@ -1355,13 +1373,13 @@
         <v>0.45669599999999999</v>
       </c>
       <c r="G9">
-        <v>38109.061999999998</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>38386.188000000002</v>
+        <v>57</v>
       </c>
       <c r="I9">
-        <v>38748.921999999999</v>
+        <v>107</v>
       </c>
       <c r="J9" s="1">
         <v>45006</v>
@@ -1370,7 +1388,7 @@
         <v>0.77284722222222224</v>
       </c>
       <c r="L9">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="M9" s="1">
         <v>45006</v>
@@ -1420,7 +1438,7 @@
         <v>39</v>
       </c>
       <c r="D10">
-        <v>2023</v>
+        <v>208</v>
       </c>
       <c r="E10">
         <v>6.0800000000000003E-4</v>
@@ -1429,13 +1447,13 @@
         <v>0.45669599999999999</v>
       </c>
       <c r="G10">
-        <v>38109.061999999998</v>
+        <v>9</v>
       </c>
       <c r="H10">
-        <v>38386.188000000002</v>
+        <v>58</v>
       </c>
       <c r="I10">
-        <v>38748.921999999999</v>
+        <v>108</v>
       </c>
       <c r="J10" s="1">
         <v>45007</v>
@@ -1444,7 +1462,7 @@
         <v>0.81451388888888898</v>
       </c>
       <c r="L10">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="M10" s="1">
         <v>45007</v>
@@ -1494,7 +1512,7 @@
         <v>41</v>
       </c>
       <c r="D11">
-        <v>2023</v>
+        <v>209</v>
       </c>
       <c r="E11">
         <v>6.1700000000000004E-4</v>
@@ -1503,13 +1521,13 @@
         <v>7.2839840000000002</v>
       </c>
       <c r="G11">
-        <v>38419.745999999999</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>39588.582000000002</v>
+        <v>59</v>
       </c>
       <c r="I11">
-        <v>43270.995999999999</v>
+        <v>109</v>
       </c>
       <c r="J11" s="1">
         <v>45006</v>
@@ -1518,7 +1536,7 @@
         <v>0.77246527777777774</v>
       </c>
       <c r="L11">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="M11" s="1">
         <v>45006</v>
@@ -1560,77 +1578,77 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D12">
-        <v>2023</v>
-      </c>
-      <c r="E12">
+        <v>210</v>
+      </c>
+      <c r="E12" s="8">
         <v>7.7899890000000003</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>1.9509620000000001</v>
       </c>
       <c r="G12">
-        <v>38322.644999999997</v>
+        <v>11</v>
       </c>
       <c r="H12">
-        <v>38772.641000000003</v>
+        <v>60</v>
       </c>
       <c r="I12">
-        <v>39577.230000000003</v>
-      </c>
-      <c r="J12" s="1">
-        <v>45006</v>
-      </c>
-      <c r="K12" s="2">
+        <v>110</v>
+      </c>
+      <c r="J12" s="9">
+        <v>45006</v>
+      </c>
+      <c r="K12" s="10">
         <v>0.77255542824074075</v>
       </c>
       <c r="L12">
-        <v>18</v>
-      </c>
-      <c r="M12" s="1">
-        <v>45006</v>
-      </c>
-      <c r="N12" s="2">
+        <v>11</v>
+      </c>
+      <c r="M12" s="9">
+        <v>45006</v>
+      </c>
+      <c r="N12" s="10">
         <v>0.27255542824074075</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="8">
         <v>6</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
+      <c r="Q12" s="8">
+        <v>0</v>
+      </c>
+      <c r="S12" s="8">
+        <v>0</v>
+      </c>
+      <c r="U12" s="8">
+        <v>0</v>
+      </c>
+      <c r="V12" s="8">
         <v>1</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W12" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="X12" s="4">
+      <c r="X12" s="11">
         <v>-27.524301000000001</v>
       </c>
-      <c r="Y12" s="6">
+      <c r="Y12" s="12">
         <v>153.49443199999999</v>
       </c>
-      <c r="Z12" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB12" t="s">
+      <c r="Z12" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB12" s="8" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1642,7 +1660,7 @@
         <v>43</v>
       </c>
       <c r="D13">
-        <v>2023</v>
+        <v>211</v>
       </c>
       <c r="E13">
         <v>5.6999999999999998E-4</v>
@@ -1651,13 +1669,13 @@
         <v>2.0192320000000001</v>
       </c>
       <c r="G13">
-        <v>37622.050999999999</v>
+        <v>12</v>
       </c>
       <c r="H13">
-        <v>38403.671999999999</v>
+        <v>61</v>
       </c>
       <c r="I13">
-        <v>40059.120999999999</v>
+        <v>111</v>
       </c>
       <c r="J13" s="1">
         <v>45006</v>
@@ -1666,7 +1684,7 @@
         <v>0.77353009259259264</v>
       </c>
       <c r="L13">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="M13" s="1">
         <v>45006</v>
@@ -1716,7 +1734,7 @@
         <v>43</v>
       </c>
       <c r="D14">
-        <v>2023</v>
+        <v>212</v>
       </c>
       <c r="E14">
         <v>2.63219</v>
@@ -1725,13 +1743,13 @@
         <v>2.4880469999999999</v>
       </c>
       <c r="G14">
-        <v>38423.633000000002</v>
+        <v>13</v>
       </c>
       <c r="H14">
-        <v>40127.480000000003</v>
+        <v>62</v>
       </c>
       <c r="I14">
-        <v>46220.620999999999</v>
+        <v>112</v>
       </c>
       <c r="J14" s="1">
         <v>45006</v>
@@ -1740,7 +1758,7 @@
         <v>0.77356054398148144</v>
       </c>
       <c r="L14">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="M14" s="1">
         <v>45006</v>
@@ -1790,7 +1808,7 @@
         <v>43</v>
       </c>
       <c r="D15">
-        <v>2023</v>
+        <v>213</v>
       </c>
       <c r="E15">
         <v>5.6901440000000001</v>
@@ -1799,13 +1817,13 @@
         <v>1.5416270000000001</v>
       </c>
       <c r="G15">
-        <v>38147.879000000001</v>
+        <v>14</v>
       </c>
       <c r="H15">
-        <v>38685.828000000001</v>
+        <v>63</v>
       </c>
       <c r="I15">
-        <v>39683.370999999999</v>
+        <v>113</v>
       </c>
       <c r="J15" s="1">
         <v>45006</v>
@@ -1814,7 +1832,7 @@
         <v>0.7735959375</v>
       </c>
       <c r="L15">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="M15" s="1">
         <v>45006</v>
@@ -1864,7 +1882,7 @@
         <v>43</v>
       </c>
       <c r="D16">
-        <v>2023</v>
+        <v>214</v>
       </c>
       <c r="E16">
         <v>8.6172989999999992</v>
@@ -1873,13 +1891,13 @@
         <v>3.8527939999999998</v>
       </c>
       <c r="G16">
-        <v>38246.535000000003</v>
+        <v>15</v>
       </c>
       <c r="H16">
-        <v>38756.894999999997</v>
+        <v>64</v>
       </c>
       <c r="I16">
-        <v>39645.737999999998</v>
+        <v>114</v>
       </c>
       <c r="J16" s="1">
         <v>45006</v>
@@ -1888,7 +1906,7 @@
         <v>0.77362982638888889</v>
       </c>
       <c r="L16">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="M16" s="1">
         <v>45006</v>
@@ -1938,7 +1956,7 @@
         <v>45</v>
       </c>
       <c r="D17">
-        <v>2023</v>
+        <v>215</v>
       </c>
       <c r="E17">
         <v>5.7899999999999998E-4</v>
@@ -1947,13 +1965,13 @@
         <v>5.3369450000000001</v>
       </c>
       <c r="G17">
-        <v>37485.061999999998</v>
+        <v>16</v>
       </c>
       <c r="H17">
-        <v>38690.402000000002</v>
+        <v>65</v>
       </c>
       <c r="I17">
-        <v>42695.042999999998</v>
+        <v>115</v>
       </c>
       <c r="J17" s="1">
         <v>45006</v>
@@ -1962,7 +1980,7 @@
         <v>0.77377314814814813</v>
       </c>
       <c r="L17">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M17" s="1">
         <v>45006</v>
@@ -2012,7 +2030,7 @@
         <v>45</v>
       </c>
       <c r="D18">
-        <v>2023</v>
+        <v>216</v>
       </c>
       <c r="E18">
         <v>6.0062069999999999</v>
@@ -2021,13 +2039,13 @@
         <v>2.7681170000000002</v>
       </c>
       <c r="G18">
-        <v>37697.339999999997</v>
+        <v>17</v>
       </c>
       <c r="H18">
-        <v>38782.883000000002</v>
+        <v>66</v>
       </c>
       <c r="I18">
-        <v>41130.906000000003</v>
+        <v>116</v>
       </c>
       <c r="J18" s="1">
         <v>45006</v>
@@ -2036,7 +2054,7 @@
         <v>0.773842662037037</v>
       </c>
       <c r="L18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M18" s="1">
         <v>45006</v>
@@ -2086,7 +2104,7 @@
         <v>45</v>
       </c>
       <c r="D19">
-        <v>2023</v>
+        <v>217</v>
       </c>
       <c r="E19">
         <v>9.3170940000000009</v>
@@ -2095,13 +2113,13 @@
         <v>0.14712500000000001</v>
       </c>
       <c r="G19">
-        <v>39217.57</v>
+        <v>18</v>
       </c>
       <c r="H19">
-        <v>40080.148000000001</v>
+        <v>67</v>
       </c>
       <c r="I19">
-        <v>42159.699000000001</v>
+        <v>117</v>
       </c>
       <c r="J19" s="1">
         <v>45006</v>
@@ -2160,7 +2178,7 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <v>2023</v>
+        <v>218</v>
       </c>
       <c r="E20">
         <v>9.9732800000000008</v>
@@ -2169,13 +2187,13 @@
         <v>0.208761</v>
       </c>
       <c r="G20">
-        <v>37744.25</v>
+        <v>19</v>
       </c>
       <c r="H20">
-        <v>38510.5</v>
+        <v>68</v>
       </c>
       <c r="I20">
-        <v>41054.633000000002</v>
+        <v>118</v>
       </c>
       <c r="J20" s="1">
         <v>45006</v>
@@ -2184,7 +2202,7 @@
         <v>0.77388856481481472</v>
       </c>
       <c r="L20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M20" s="1">
         <v>45006</v>
@@ -2234,7 +2252,7 @@
         <v>45</v>
       </c>
       <c r="D21">
-        <v>2023</v>
+        <v>219</v>
       </c>
       <c r="E21">
         <v>10.844884</v>
@@ -2243,13 +2261,13 @@
         <v>0.66497799999999996</v>
       </c>
       <c r="G21">
-        <v>37145.925999999999</v>
+        <v>20</v>
       </c>
       <c r="H21">
-        <v>38009.754000000001</v>
+        <v>69</v>
       </c>
       <c r="I21">
-        <v>39911.855000000003</v>
+        <v>119</v>
       </c>
       <c r="J21" s="1">
         <v>45006</v>
@@ -2258,7 +2276,7 @@
         <v>0.77389865740740738</v>
       </c>
       <c r="L21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M21" s="1">
         <v>45006</v>
@@ -2308,7 +2326,7 @@
         <v>47</v>
       </c>
       <c r="D22">
-        <v>2023</v>
+        <v>220</v>
       </c>
       <c r="E22">
         <v>6.2100000000000002E-4</v>
@@ -2317,13 +2335,13 @@
         <v>0.307255</v>
       </c>
       <c r="G22">
-        <v>38424.226999999999</v>
+        <v>21</v>
       </c>
       <c r="H22">
-        <v>39511.108999999997</v>
+        <v>70</v>
       </c>
       <c r="I22">
-        <v>42529.434000000001</v>
+        <v>120</v>
       </c>
       <c r="J22" s="1">
         <v>45006</v>
@@ -2332,7 +2350,7 @@
         <v>0.77401620370370372</v>
       </c>
       <c r="L22">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="M22" s="1">
         <v>45006</v>
@@ -2382,7 +2400,7 @@
         <v>47</v>
       </c>
       <c r="D23">
-        <v>2023</v>
+        <v>221</v>
       </c>
       <c r="E23">
         <v>2.2334670000000001</v>
@@ -2391,13 +2409,13 @@
         <v>1.633637</v>
       </c>
       <c r="G23">
-        <v>38947.781000000003</v>
+        <v>22</v>
       </c>
       <c r="H23">
-        <v>39582.714999999997</v>
+        <v>71</v>
       </c>
       <c r="I23">
-        <v>40718.800999999999</v>
+        <v>121</v>
       </c>
       <c r="J23" s="1">
         <v>45006</v>
@@ -2406,7 +2424,7 @@
         <v>0.77404203703703711</v>
       </c>
       <c r="L23">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="M23" s="1">
         <v>45006</v>
@@ -2456,7 +2474,7 @@
         <v>49</v>
       </c>
       <c r="D24">
-        <v>2023</v>
+        <v>222</v>
       </c>
       <c r="E24">
         <v>6.0700000000000001E-4</v>
@@ -2465,13 +2483,13 @@
         <v>0.78392399999999995</v>
       </c>
       <c r="G24">
-        <v>38523.785000000003</v>
+        <v>23</v>
       </c>
       <c r="H24">
-        <v>39978.938000000002</v>
+        <v>72</v>
       </c>
       <c r="I24">
-        <v>44100.347999999998</v>
+        <v>122</v>
       </c>
       <c r="J24" s="1">
         <v>45006</v>
@@ -2480,7 +2498,7 @@
         <v>0.77427083333333335</v>
       </c>
       <c r="L24">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="M24" s="1">
         <v>45006</v>
@@ -2530,7 +2548,7 @@
         <v>49</v>
       </c>
       <c r="D25">
-        <v>2023</v>
+        <v>223</v>
       </c>
       <c r="E25">
         <v>1.562287</v>
@@ -2539,13 +2557,13 @@
         <v>1.8582339999999999</v>
       </c>
       <c r="G25">
-        <v>36410.531000000003</v>
+        <v>24</v>
       </c>
       <c r="H25">
-        <v>37342.101999999999</v>
+        <v>73</v>
       </c>
       <c r="I25">
-        <v>39298.625</v>
+        <v>123</v>
       </c>
       <c r="J25" s="1">
         <v>45006</v>
@@ -2554,7 +2572,7 @@
         <v>0.77428890046296295</v>
       </c>
       <c r="L25">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M25" s="1">
         <v>45006</v>
@@ -2604,7 +2622,7 @@
         <v>51</v>
       </c>
       <c r="D26">
-        <v>2023</v>
+        <v>224</v>
       </c>
       <c r="E26">
         <v>6.2699999999999995E-4</v>
@@ -2613,13 +2631,13 @@
         <v>7.5561439999999997</v>
       </c>
       <c r="G26">
-        <v>31872.213</v>
+        <v>25</v>
       </c>
       <c r="H26">
-        <v>33355.839999999997</v>
+        <v>74</v>
       </c>
       <c r="I26">
-        <v>38321.648000000001</v>
+        <v>124</v>
       </c>
       <c r="J26" s="1">
         <v>45006</v>
@@ -2628,7 +2646,7 @@
         <v>0.77413194444444444</v>
       </c>
       <c r="L26">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M26" s="1">
         <v>45006</v>
@@ -2678,7 +2696,7 @@
         <v>51</v>
       </c>
       <c r="D27">
-        <v>2023</v>
+        <v>225</v>
       </c>
       <c r="E27">
         <v>8.0887220000000006</v>
@@ -2687,13 +2705,13 @@
         <v>1.9795959999999999</v>
       </c>
       <c r="G27">
-        <v>37602.648000000001</v>
+        <v>26</v>
       </c>
       <c r="H27">
-        <v>38521.065999999999</v>
+        <v>75</v>
       </c>
       <c r="I27">
-        <v>41025.038999999997</v>
+        <v>125</v>
       </c>
       <c r="J27" s="1">
         <v>45006</v>
@@ -2702,7 +2720,7 @@
         <v>0.77422555555555561</v>
       </c>
       <c r="L27">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="M27" s="1">
         <v>45006</v>
@@ -2752,7 +2770,7 @@
         <v>53</v>
       </c>
       <c r="D28">
-        <v>2023</v>
+        <v>226</v>
       </c>
       <c r="E28">
         <v>6.1700000000000004E-4</v>
@@ -2761,13 +2779,13 @@
         <v>1.595985</v>
       </c>
       <c r="G28">
-        <v>36878.516000000003</v>
+        <v>27</v>
       </c>
       <c r="H28">
-        <v>37472.663999999997</v>
+        <v>76</v>
       </c>
       <c r="I28">
-        <v>38312.586000000003</v>
+        <v>126</v>
       </c>
       <c r="J28" s="1">
         <v>45006</v>
@@ -2776,7 +2794,7 @@
         <v>0.77515046296296297</v>
       </c>
       <c r="L28">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="M28" s="1">
         <v>45006</v>
@@ -2826,7 +2844,7 @@
         <v>55</v>
       </c>
       <c r="D29">
-        <v>2023</v>
+        <v>227</v>
       </c>
       <c r="E29">
         <v>6.4300000000000002E-4</v>
@@ -2835,13 +2853,13 @@
         <v>1.261404</v>
       </c>
       <c r="G29">
-        <v>37643.038999999997</v>
+        <v>28</v>
       </c>
       <c r="H29">
-        <v>38655.421999999999</v>
+        <v>77</v>
       </c>
       <c r="I29">
-        <v>41584.199000000001</v>
+        <v>127</v>
       </c>
       <c r="J29" s="1">
         <v>45006</v>
@@ -2850,7 +2868,7 @@
         <v>0.77434027777777781</v>
       </c>
       <c r="L29">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="M29" s="1">
         <v>45006</v>
@@ -2900,7 +2918,7 @@
         <v>53</v>
       </c>
       <c r="D30">
-        <v>2023</v>
+        <v>228</v>
       </c>
       <c r="E30">
         <v>2.4486569999999999</v>
@@ -2909,13 +2927,13 @@
         <v>0.43772699999999998</v>
       </c>
       <c r="G30">
-        <v>36281.733999999997</v>
+        <v>29</v>
       </c>
       <c r="H30">
-        <v>36575.438000000002</v>
+        <v>78</v>
       </c>
       <c r="I30">
-        <v>37567.866999999998</v>
+        <v>128</v>
       </c>
       <c r="J30" s="1">
         <v>45006</v>
@@ -2924,7 +2942,7 @@
         <v>0.77517879629629638</v>
       </c>
       <c r="L30">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="M30" s="1">
         <v>45006</v>
@@ -2974,7 +2992,7 @@
         <v>55</v>
       </c>
       <c r="D31">
-        <v>2023</v>
+        <v>229</v>
       </c>
       <c r="E31">
         <v>3.2873950000000001</v>
@@ -2983,13 +3001,13 @@
         <v>11.648963</v>
       </c>
       <c r="G31">
-        <v>36343.144999999997</v>
+        <v>30</v>
       </c>
       <c r="H31">
-        <v>37827.285000000003</v>
+        <v>79</v>
       </c>
       <c r="I31">
-        <v>42294.586000000003</v>
+        <v>129</v>
       </c>
       <c r="J31" s="1">
         <v>45006</v>
@@ -2998,7 +3016,7 @@
         <v>0.7743783101851851</v>
       </c>
       <c r="L31">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="M31" s="1">
         <v>45006</v>
@@ -3048,7 +3066,7 @@
         <v>57</v>
       </c>
       <c r="D32">
-        <v>2023</v>
+        <v>230</v>
       </c>
       <c r="E32">
         <v>0.11736199999999999</v>
@@ -3057,13 +3075,13 @@
         <v>3.9850910000000002</v>
       </c>
       <c r="G32">
-        <v>38893.269999999997</v>
+        <v>31</v>
       </c>
       <c r="H32">
-        <v>40312.550999999999</v>
+        <v>80</v>
       </c>
       <c r="I32">
-        <v>45016.855000000003</v>
+        <v>130</v>
       </c>
       <c r="J32" s="1">
         <v>45006</v>
@@ -3072,7 +3090,7 @@
         <v>0.77466570601851847</v>
       </c>
       <c r="L32">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="M32" s="1">
         <v>45006</v>
@@ -3122,7 +3140,7 @@
         <v>57</v>
       </c>
       <c r="D33">
-        <v>2023</v>
+        <v>231</v>
       </c>
       <c r="E33">
         <v>4.930466</v>
@@ -3131,13 +3149,13 @@
         <v>1.511995</v>
       </c>
       <c r="G33">
-        <v>38970.898000000001</v>
+        <v>32</v>
       </c>
       <c r="H33">
-        <v>39760.938000000002</v>
+        <v>81</v>
       </c>
       <c r="I33">
-        <v>41729.671999999999</v>
+        <v>131</v>
       </c>
       <c r="J33" s="1">
         <v>45006</v>
@@ -3146,7 +3164,7 @@
         <v>0.77472140046296301</v>
       </c>
       <c r="L33">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="M33" s="1">
         <v>45006</v>
@@ -3196,7 +3214,7 @@
         <v>59</v>
       </c>
       <c r="D34">
-        <v>2023</v>
+        <v>232</v>
       </c>
       <c r="E34">
         <v>6.0999999999999997E-4</v>
@@ -3205,13 +3223,13 @@
         <v>1.027946</v>
       </c>
       <c r="G34">
-        <v>38783.519999999997</v>
+        <v>33</v>
       </c>
       <c r="H34">
-        <v>40494.105000000003</v>
+        <v>82</v>
       </c>
       <c r="I34">
-        <v>43816.406000000003</v>
+        <v>132</v>
       </c>
       <c r="J34" s="1">
         <v>45006</v>
@@ -3220,7 +3238,7 @@
         <v>0.77528935185185188</v>
       </c>
       <c r="L34">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="M34" s="1">
         <v>45006</v>
@@ -3270,7 +3288,7 @@
         <v>61</v>
       </c>
       <c r="D35">
-        <v>2023</v>
+        <v>233</v>
       </c>
       <c r="E35">
         <v>5.3899999999999998E-4</v>
@@ -3279,13 +3297,13 @@
         <v>6.9087589999999999</v>
       </c>
       <c r="G35">
-        <v>38010.616999999998</v>
+        <v>34</v>
       </c>
       <c r="H35">
-        <v>39346.391000000003</v>
+        <v>83</v>
       </c>
       <c r="I35">
-        <v>44403.75</v>
+        <v>133</v>
       </c>
       <c r="J35" s="1">
         <v>45006</v>
@@ -3294,7 +3312,7 @@
         <v>0.77453703703703702</v>
       </c>
       <c r="L35">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="M35" s="1">
         <v>45006</v>
@@ -3344,7 +3362,7 @@
         <v>63</v>
       </c>
       <c r="D36">
-        <v>2023</v>
+        <v>234</v>
       </c>
       <c r="E36">
         <v>5.8699999999999996E-4</v>
@@ -3353,13 +3371,13 @@
         <v>3.2025510000000001</v>
       </c>
       <c r="G36">
-        <v>37454.171999999999</v>
+        <v>35</v>
       </c>
       <c r="H36">
-        <v>37972.512000000002</v>
+        <v>84</v>
       </c>
       <c r="I36">
-        <v>38987.773000000001</v>
+        <v>134</v>
       </c>
       <c r="J36" s="1">
         <v>45006</v>
@@ -3368,7 +3386,7 @@
         <v>0.77498842592592587</v>
       </c>
       <c r="L36">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="M36" s="1">
         <v>45006</v>
@@ -3418,7 +3436,7 @@
         <v>63</v>
       </c>
       <c r="D37">
-        <v>2023</v>
+        <v>235</v>
       </c>
       <c r="E37">
         <v>4.6572630000000004</v>
@@ -3427,10 +3445,10 @@
         <v>1.2144330000000001</v>
       </c>
       <c r="G37">
-        <v>39143.324000000001</v>
+        <v>36</v>
       </c>
       <c r="H37">
-        <v>39924.796999999999</v>
+        <v>85</v>
       </c>
       <c r="I37">
         <v>41722.637000000002</v>
@@ -3442,7 +3460,7 @@
         <v>0.77504232638888892</v>
       </c>
       <c r="L37">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="M37" s="1">
         <v>45006</v>
@@ -3492,7 +3510,7 @@
         <v>63</v>
       </c>
       <c r="D38">
-        <v>2023</v>
+        <v>236</v>
       </c>
       <c r="E38">
         <v>6.913869</v>
@@ -3501,10 +3519,10 @@
         <v>2.268497</v>
       </c>
       <c r="G38">
-        <v>36349.156000000003</v>
+        <v>37</v>
       </c>
       <c r="H38">
-        <v>37203.875</v>
+        <v>86</v>
       </c>
       <c r="I38">
         <v>38837.214999999997</v>
@@ -3516,7 +3534,7 @@
         <v>0.77506843749999998</v>
       </c>
       <c r="L38">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="M38" s="1">
         <v>45006</v>
@@ -3564,11 +3582,951 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6550273E-603A-42D8-A18D-89926B99F639}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>200</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="3">
+        <v>6.4872685185185186E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>201</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>101</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.1025462962962963</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>202</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>102</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.14721064814814816</v>
+      </c>
+      <c r="F4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>203</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>103</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.19451388888888888</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>203</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>103</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.19451388888888888</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>204</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>54</v>
+      </c>
+      <c r="D7">
+        <v>104</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.23162037037037037</v>
+      </c>
+      <c r="F7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>204</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <v>104</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.23162037037037037</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>205</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <v>105</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.27392361111111113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>206</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>106</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.31562499999999999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>207</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>57</v>
+      </c>
+      <c r="D11">
+        <v>107</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.35618055555555556</v>
+      </c>
+      <c r="F11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>208</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>108</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.39784722222222224</v>
+      </c>
+      <c r="F12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>209</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>59</v>
+      </c>
+      <c r="D13">
+        <v>109</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.43913194444444442</v>
+      </c>
+      <c r="F13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>210</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>110</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.48087962962962966</v>
+      </c>
+      <c r="F14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>211</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>111</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.52353009259259264</v>
+      </c>
+      <c r="F15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>212</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>62</v>
+      </c>
+      <c r="D16">
+        <v>112</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.56521990740740746</v>
+      </c>
+      <c r="F16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>213</v>
+      </c>
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>63</v>
+      </c>
+      <c r="D17">
+        <v>113</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.60692129629629632</v>
+      </c>
+      <c r="F17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>214</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>64</v>
+      </c>
+      <c r="D18">
+        <v>114</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.64862268518518518</v>
+      </c>
+      <c r="F18" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>215</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>65</v>
+      </c>
+      <c r="D19">
+        <v>115</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.69043981481481487</v>
+      </c>
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>216</v>
+      </c>
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>66</v>
+      </c>
+      <c r="D20">
+        <v>116</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.73217592592592595</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>217</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>67</v>
+      </c>
+      <c r="D21">
+        <v>117</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.77387731481481481</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>218</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>68</v>
+      </c>
+      <c r="D22">
+        <v>118</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.81555555555555559</v>
+      </c>
+      <c r="F22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>219</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>119</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.85722222222222222</v>
+      </c>
+      <c r="F23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>220</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>70</v>
+      </c>
+      <c r="D24">
+        <v>120</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.89901620370370372</v>
+      </c>
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>221</v>
+      </c>
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>71</v>
+      </c>
+      <c r="D25">
+        <v>121</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.94070601851851854</v>
+      </c>
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>222</v>
+      </c>
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>72</v>
+      </c>
+      <c r="D26">
+        <v>122</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.98260416666666661</v>
+      </c>
+      <c r="F26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>223</v>
+      </c>
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>73</v>
+      </c>
+      <c r="D27">
+        <v>123</v>
+      </c>
+      <c r="E27" s="13">
+        <v>1.0242824074074075</v>
+      </c>
+      <c r="F27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>224</v>
+      </c>
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>74</v>
+      </c>
+      <c r="D28">
+        <v>124</v>
+      </c>
+      <c r="E28" s="13">
+        <v>1.0657986111111111</v>
+      </c>
+      <c r="F28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>225</v>
+      </c>
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>75</v>
+      </c>
+      <c r="D29">
+        <v>125</v>
+      </c>
+      <c r="E29" s="13">
+        <v>1.1075578703703703</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>226</v>
+      </c>
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="C30">
+        <v>76</v>
+      </c>
+      <c r="D30">
+        <v>126</v>
+      </c>
+      <c r="E30" s="13">
+        <v>1.1501504629629629</v>
+      </c>
+      <c r="F30" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>227</v>
+      </c>
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>77</v>
+      </c>
+      <c r="D31">
+        <v>127</v>
+      </c>
+      <c r="E31" s="13">
+        <v>1.1910069444444444</v>
+      </c>
+      <c r="F31" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>228</v>
+      </c>
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>78</v>
+      </c>
+      <c r="D32">
+        <v>128</v>
+      </c>
+      <c r="E32" s="13">
+        <v>1.2335069444444444</v>
+      </c>
+      <c r="F32" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>229</v>
+      </c>
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>79</v>
+      </c>
+      <c r="D33">
+        <v>129</v>
+      </c>
+      <c r="E33" s="13">
+        <v>1.274375</v>
+      </c>
+      <c r="F33" t="s">
+        <v>93</v>
+      </c>
+      <c r="G33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>230</v>
+      </c>
+      <c r="B34">
+        <v>31</v>
+      </c>
+      <c r="C34">
+        <v>80</v>
+      </c>
+      <c r="D34">
+        <v>130</v>
+      </c>
+      <c r="E34" s="13">
+        <v>1.3163310185185184</v>
+      </c>
+      <c r="F34" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>231</v>
+      </c>
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>81</v>
+      </c>
+      <c r="D35">
+        <v>131</v>
+      </c>
+      <c r="E35" s="13">
+        <v>1.3580439814814815</v>
+      </c>
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>232</v>
+      </c>
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <v>82</v>
+      </c>
+      <c r="D36">
+        <v>132</v>
+      </c>
+      <c r="E36" s="13">
+        <v>1.4002893518518518</v>
+      </c>
+      <c r="F36" t="s">
+        <v>99</v>
+      </c>
+      <c r="G36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>233</v>
+      </c>
+      <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>83</v>
+      </c>
+      <c r="D37">
+        <v>133</v>
+      </c>
+      <c r="E37" s="13">
+        <v>1.4412037037037038</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>234</v>
+      </c>
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <v>84</v>
+      </c>
+      <c r="D38">
+        <v>134</v>
+      </c>
+      <c r="E38" s="13">
+        <v>1.4833217592592594</v>
+      </c>
+      <c r="F38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>235</v>
+      </c>
+      <c r="B39">
+        <v>36</v>
+      </c>
+      <c r="C39">
+        <v>85</v>
+      </c>
+      <c r="D39">
+        <v>41722.637000000002</v>
+      </c>
+      <c r="E39" s="13">
+        <v>1.5250347222222222</v>
+      </c>
+      <c r="F39" t="s">
+        <v>97</v>
+      </c>
+      <c r="G39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>236</v>
+      </c>
+      <c r="B40">
+        <v>37</v>
+      </c>
+      <c r="C40">
+        <v>86</v>
+      </c>
+      <c r="D40">
+        <v>38837.214999999997</v>
+      </c>
+      <c r="E40" s="13">
+        <v>1.5667245370370371</v>
+      </c>
+      <c r="F40" t="s">
+        <v>103</v>
+      </c>
+      <c r="G40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7CA6A7A-4D1B-4018-8718-C48A1CCF3A8E}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A12" sqref="A12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3734,23 +4692,26 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2023</v>
+      </c>
       <c r="B7">
-        <v>43204.55</v>
+        <v>34144.305</v>
       </c>
       <c r="C7">
-        <v>40000.050000000003</v>
+        <v>35101.711000000003</v>
       </c>
       <c r="D7">
-        <v>42666.25</v>
+        <v>37318.620999999999</v>
       </c>
       <c r="E7" s="3">
-        <v>18</v>
+        <v>0.77328703703703705</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="H7" t="s">
         <v>109</v>
@@ -3773,7 +4734,7 @@
         <v>0.77328703703703705</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="G8" t="s">
         <v>77</v>
@@ -3787,25 +4748,25 @@
         <v>2023</v>
       </c>
       <c r="B9">
-        <v>34144.305</v>
+        <v>39698.879000000001</v>
       </c>
       <c r="C9">
-        <v>35101.711000000003</v>
+        <v>40574.574000000001</v>
       </c>
       <c r="D9">
-        <v>37318.620999999999</v>
+        <v>43022.491999999998</v>
       </c>
       <c r="E9" s="3">
-        <v>0.77328703703703705</v>
+        <v>0.77392361111111108</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" t="s">
         <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3813,25 +4774,25 @@
         <v>2023</v>
       </c>
       <c r="B10">
-        <v>39698.879000000001</v>
+        <v>38716.445</v>
       </c>
       <c r="C10">
-        <v>40574.574000000001</v>
+        <v>39157.836000000003</v>
       </c>
       <c r="D10">
-        <v>43022.491999999998</v>
+        <v>40274.858999999997</v>
       </c>
       <c r="E10" s="3">
-        <v>0.77392361111111108</v>
+        <v>0.7739583333333333</v>
       </c>
       <c r="F10" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="G10" t="s">
         <v>77</v>
       </c>
       <c r="H10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3839,19 +4800,19 @@
         <v>2023</v>
       </c>
       <c r="B11">
-        <v>38716.445</v>
+        <v>38109.061999999998</v>
       </c>
       <c r="C11">
-        <v>39157.836000000003</v>
+        <v>38386.188000000002</v>
       </c>
       <c r="D11">
-        <v>40274.858999999997</v>
+        <v>38748.921999999999</v>
       </c>
       <c r="E11" s="3">
-        <v>0.7739583333333333</v>
+        <v>0.77284722222222224</v>
       </c>
       <c r="F11" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s">
         <v>77</v>
@@ -3865,19 +4826,19 @@
         <v>2023</v>
       </c>
       <c r="B12">
-        <v>38109.061999999998</v>
+        <v>38419.745999999999</v>
       </c>
       <c r="C12">
-        <v>38386.188000000002</v>
+        <v>39588.582000000002</v>
       </c>
       <c r="D12">
-        <v>38748.921999999999</v>
+        <v>43270.995999999999</v>
       </c>
       <c r="E12" s="3">
-        <v>0.77284722222222224</v>
+        <v>0.77246527777777774</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G12" t="s">
         <v>77</v>
@@ -3891,19 +4852,19 @@
         <v>2023</v>
       </c>
       <c r="B13">
-        <v>38419.745999999999</v>
+        <v>38322.644999999997</v>
       </c>
       <c r="C13">
-        <v>39588.582000000002</v>
+        <v>38772.641000000003</v>
       </c>
       <c r="D13">
-        <v>43270.995999999999</v>
+        <v>39577.230000000003</v>
       </c>
       <c r="E13" s="3">
-        <v>0.77246527777777774</v>
+        <v>0.77254629629629634</v>
       </c>
       <c r="F13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G13" t="s">
         <v>77</v>
@@ -3917,25 +4878,25 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>38322.644999999997</v>
+        <v>37622.050999999999</v>
       </c>
       <c r="C14">
-        <v>38772.641000000003</v>
+        <v>38403.671999999999</v>
       </c>
       <c r="D14">
-        <v>39577.230000000003</v>
+        <v>40059.120999999999</v>
       </c>
       <c r="E14" s="3">
-        <v>0.77254629629629634</v>
+        <v>0.77353009259259264</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G14" t="s">
         <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -3943,25 +4904,25 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>37622.050999999999</v>
+        <v>38423.633000000002</v>
       </c>
       <c r="C15">
-        <v>38403.671999999999</v>
+        <v>40127.480000000003</v>
       </c>
       <c r="D15">
-        <v>40059.120999999999</v>
+        <v>46220.620999999999</v>
       </c>
       <c r="E15" s="3">
-        <v>0.77353009259259264</v>
+        <v>0.77355324074074072</v>
       </c>
       <c r="F15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G15" t="s">
         <v>77</v>
       </c>
       <c r="H15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -3969,19 +4930,19 @@
         <v>2023</v>
       </c>
       <c r="B16">
-        <v>38423.633000000002</v>
+        <v>38147.879000000001</v>
       </c>
       <c r="C16">
-        <v>40127.480000000003</v>
+        <v>38685.828000000001</v>
       </c>
       <c r="D16">
-        <v>46220.620999999999</v>
+        <v>39683.370999999999</v>
       </c>
       <c r="E16" s="3">
-        <v>0.77355324074074072</v>
+        <v>0.77358796296296295</v>
       </c>
       <c r="F16" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
         <v>77</v>
@@ -3995,19 +4956,19 @@
         <v>2023</v>
       </c>
       <c r="B17">
-        <v>38147.879000000001</v>
+        <v>38246.535000000003</v>
       </c>
       <c r="C17">
-        <v>38685.828000000001</v>
+        <v>38756.894999999997</v>
       </c>
       <c r="D17">
-        <v>39683.370999999999</v>
+        <v>39645.737999999998</v>
       </c>
       <c r="E17" s="3">
-        <v>0.77358796296296295</v>
+        <v>0.77362268518518518</v>
       </c>
       <c r="F17" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="G17" t="s">
         <v>77</v>
@@ -4021,25 +4982,25 @@
         <v>2023</v>
       </c>
       <c r="B18">
-        <v>38246.535000000003</v>
+        <v>37485.061999999998</v>
       </c>
       <c r="C18">
-        <v>38756.894999999997</v>
+        <v>38690.402000000002</v>
       </c>
       <c r="D18">
-        <v>39645.737999999998</v>
+        <v>42695.042999999998</v>
       </c>
       <c r="E18" s="3">
-        <v>0.77362268518518518</v>
+        <v>0.77377314814814813</v>
       </c>
       <c r="F18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G18" t="s">
         <v>77</v>
       </c>
       <c r="H18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -4047,25 +5008,25 @@
         <v>2023</v>
       </c>
       <c r="B19">
-        <v>37485.061999999998</v>
+        <v>37697.339999999997</v>
       </c>
       <c r="C19">
-        <v>38690.402000000002</v>
+        <v>38782.883000000002</v>
       </c>
       <c r="D19">
-        <v>42695.042999999998</v>
+        <v>41130.906000000003</v>
       </c>
       <c r="E19" s="3">
-        <v>0.77377314814814813</v>
+        <v>0.77384259259259258</v>
       </c>
       <c r="F19" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="G19" t="s">
         <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4073,25 +5034,25 @@
         <v>2023</v>
       </c>
       <c r="B20">
-        <v>37697.339999999997</v>
+        <v>39217.57</v>
       </c>
       <c r="C20">
-        <v>38782.883000000002</v>
+        <v>40080.148000000001</v>
       </c>
       <c r="D20">
-        <v>41130.906000000003</v>
+        <v>42159.699000000001</v>
       </c>
       <c r="E20" s="3">
-        <v>0.77384259259259258</v>
+        <v>0.77387731481481481</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="G20" t="s">
         <v>77</v>
       </c>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -4099,25 +5060,25 @@
         <v>2023</v>
       </c>
       <c r="B21">
-        <v>39217.57</v>
+        <v>37744.25</v>
       </c>
       <c r="C21">
-        <v>40080.148000000001</v>
+        <v>38510.5</v>
       </c>
       <c r="D21">
-        <v>42159.699000000001</v>
+        <v>41054.633000000002</v>
       </c>
       <c r="E21" s="3">
-        <v>0.77387731481481481</v>
+        <v>0.77388888888888885</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G21" t="s">
         <v>77</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4125,25 +5086,25 @@
         <v>2023</v>
       </c>
       <c r="B22">
-        <v>37744.25</v>
+        <v>37145.925999999999</v>
       </c>
       <c r="C22">
-        <v>38510.5</v>
+        <v>38009.754000000001</v>
       </c>
       <c r="D22">
-        <v>41054.633000000002</v>
+        <v>39911.855000000003</v>
       </c>
       <c r="E22" s="3">
         <v>0.77388888888888885</v>
       </c>
       <c r="F22" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="G22" t="s">
         <v>77</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -4151,25 +5112,25 @@
         <v>2023</v>
       </c>
       <c r="B23">
-        <v>37145.925999999999</v>
+        <v>38424.226999999999</v>
       </c>
       <c r="C23">
-        <v>38009.754000000001</v>
+        <v>39511.108999999997</v>
       </c>
       <c r="D23">
-        <v>39911.855000000003</v>
+        <v>42529.434000000001</v>
       </c>
       <c r="E23" s="3">
-        <v>0.77388888888888885</v>
+        <v>0.77401620370370372</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="G23" t="s">
         <v>77</v>
       </c>
       <c r="H23" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4177,25 +5138,25 @@
         <v>2023</v>
       </c>
       <c r="B24">
-        <v>38424.226999999999</v>
+        <v>38947.781000000003</v>
       </c>
       <c r="C24">
-        <v>39511.108999999997</v>
+        <v>39582.714999999997</v>
       </c>
       <c r="D24">
-        <v>42529.434000000001</v>
+        <v>40718.800999999999</v>
       </c>
       <c r="E24" s="3">
-        <v>0.77401620370370372</v>
+        <v>0.7740393518518518</v>
       </c>
       <c r="F24" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
         <v>77</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4203,19 +5164,19 @@
         <v>2023</v>
       </c>
       <c r="B25">
-        <v>38947.781000000003</v>
+        <v>38523.785000000003</v>
       </c>
       <c r="C25">
-        <v>39582.714999999997</v>
+        <v>39978.938000000002</v>
       </c>
       <c r="D25">
-        <v>40718.800999999999</v>
+        <v>44100.347999999998</v>
       </c>
       <c r="E25" s="3">
-        <v>0.7740393518518518</v>
+        <v>0.77427083333333335</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G25" t="s">
         <v>77</v>
@@ -4229,25 +5190,25 @@
         <v>2023</v>
       </c>
       <c r="B26">
-        <v>38523.785000000003</v>
+        <v>36410.531000000003</v>
       </c>
       <c r="C26">
-        <v>39978.938000000002</v>
+        <v>37342.101999999999</v>
       </c>
       <c r="D26">
-        <v>44100.347999999998</v>
+        <v>39298.625</v>
       </c>
       <c r="E26" s="3">
-        <v>0.77427083333333335</v>
+        <v>0.77428240740740739</v>
       </c>
       <c r="F26" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="G26" t="s">
         <v>77</v>
       </c>
       <c r="H26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4255,25 +5216,25 @@
         <v>2023</v>
       </c>
       <c r="B27">
-        <v>36410.531000000003</v>
+        <v>31872.213</v>
       </c>
       <c r="C27">
-        <v>37342.101999999999</v>
+        <v>33355.839999999997</v>
       </c>
       <c r="D27">
-        <v>39298.625</v>
+        <v>38321.648000000001</v>
       </c>
       <c r="E27" s="3">
-        <v>0.77428240740740739</v>
+        <v>0.77413194444444444</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G27" t="s">
         <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -4281,25 +5242,25 @@
         <v>2023</v>
       </c>
       <c r="B28">
-        <v>31872.213</v>
+        <v>37602.648000000001</v>
       </c>
       <c r="C28">
-        <v>33355.839999999997</v>
+        <v>38521.065999999999</v>
       </c>
       <c r="D28">
-        <v>38321.648000000001</v>
+        <v>41025.038999999997</v>
       </c>
       <c r="E28" s="3">
-        <v>0.77413194444444444</v>
+        <v>0.77422453703703709</v>
       </c>
       <c r="F28" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="G28" t="s">
         <v>77</v>
       </c>
       <c r="H28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -4307,19 +5268,19 @@
         <v>2023</v>
       </c>
       <c r="B29">
-        <v>37602.648000000001</v>
+        <v>36878.516000000003</v>
       </c>
       <c r="C29">
-        <v>38521.065999999999</v>
+        <v>37472.663999999997</v>
       </c>
       <c r="D29">
-        <v>41025.038999999997</v>
+        <v>38312.586000000003</v>
       </c>
       <c r="E29" s="3">
-        <v>0.77422453703703709</v>
+        <v>0.77515046296296297</v>
       </c>
       <c r="F29" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="G29" t="s">
         <v>77</v>
@@ -4333,19 +5294,19 @@
         <v>2023</v>
       </c>
       <c r="B30">
-        <v>36878.516000000003</v>
+        <v>37643.038999999997</v>
       </c>
       <c r="C30">
-        <v>37472.663999999997</v>
+        <v>38655.421999999999</v>
       </c>
       <c r="D30">
-        <v>38312.586000000003</v>
+        <v>41584.199000000001</v>
       </c>
       <c r="E30" s="3">
-        <v>0.77515046296296297</v>
+        <v>0.77434027777777781</v>
       </c>
       <c r="F30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G30" t="s">
         <v>77</v>
@@ -4359,19 +5320,19 @@
         <v>2023</v>
       </c>
       <c r="B31">
-        <v>37643.038999999997</v>
+        <v>36281.733999999997</v>
       </c>
       <c r="C31">
-        <v>38655.421999999999</v>
+        <v>36575.438000000002</v>
       </c>
       <c r="D31">
-        <v>41584.199000000001</v>
+        <v>37567.866999999998</v>
       </c>
       <c r="E31" s="3">
-        <v>0.77434027777777781</v>
+        <v>0.77517361111111116</v>
       </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G31" t="s">
         <v>77</v>
@@ -4385,25 +5346,25 @@
         <v>2023</v>
       </c>
       <c r="B32">
-        <v>36281.733999999997</v>
+        <v>36343.144999999997</v>
       </c>
       <c r="C32">
-        <v>36575.438000000002</v>
+        <v>37827.285000000003</v>
       </c>
       <c r="D32">
-        <v>37567.866999999998</v>
+        <v>42294.586000000003</v>
       </c>
       <c r="E32" s="3">
-        <v>0.77517361111111116</v>
+        <v>0.77437500000000004</v>
       </c>
       <c r="F32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G32" t="s">
         <v>77</v>
       </c>
       <c r="H32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -4411,25 +5372,25 @@
         <v>2023</v>
       </c>
       <c r="B33">
-        <v>36343.144999999997</v>
+        <v>38893.269999999997</v>
       </c>
       <c r="C33">
-        <v>37827.285000000003</v>
+        <v>40312.550999999999</v>
       </c>
       <c r="D33">
-        <v>42294.586000000003</v>
+        <v>45016.855000000003</v>
       </c>
       <c r="E33" s="3">
-        <v>0.77437500000000004</v>
+        <v>0.7746643518518519</v>
       </c>
       <c r="F33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G33" t="s">
         <v>77</v>
       </c>
       <c r="H33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -4437,19 +5398,19 @@
         <v>2023</v>
       </c>
       <c r="B34">
-        <v>38893.269999999997</v>
+        <v>38970.898000000001</v>
       </c>
       <c r="C34">
-        <v>40312.550999999999</v>
+        <v>39760.938000000002</v>
       </c>
       <c r="D34">
-        <v>45016.855000000003</v>
+        <v>41729.671999999999</v>
       </c>
       <c r="E34" s="3">
-        <v>0.7746643518518519</v>
+        <v>0.77471064814814816</v>
       </c>
       <c r="F34" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="G34" t="s">
         <v>77</v>
@@ -4463,19 +5424,19 @@
         <v>2023</v>
       </c>
       <c r="B35">
-        <v>38970.898000000001</v>
+        <v>38783.519999999997</v>
       </c>
       <c r="C35">
-        <v>39760.938000000002</v>
+        <v>40494.105000000003</v>
       </c>
       <c r="D35">
-        <v>41729.671999999999</v>
+        <v>43816.406000000003</v>
       </c>
       <c r="E35" s="3">
-        <v>0.77471064814814816</v>
+        <v>0.77528935185185188</v>
       </c>
       <c r="F35" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="G35" t="s">
         <v>77</v>
@@ -4489,25 +5450,25 @@
         <v>2023</v>
       </c>
       <c r="B36">
-        <v>38783.519999999997</v>
+        <v>38010.616999999998</v>
       </c>
       <c r="C36">
-        <v>40494.105000000003</v>
+        <v>39346.391000000003</v>
       </c>
       <c r="D36">
-        <v>43816.406000000003</v>
+        <v>44403.75</v>
       </c>
       <c r="E36" s="3">
-        <v>0.77528935185185188</v>
-      </c>
-      <c r="F36" t="s">
-        <v>99</v>
+        <v>0.77453703703703702</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="G36" t="s">
         <v>77</v>
       </c>
       <c r="H36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -4515,25 +5476,25 @@
         <v>2023</v>
       </c>
       <c r="B37">
-        <v>38010.616999999998</v>
+        <v>37454.171999999999</v>
       </c>
       <c r="C37">
-        <v>39346.391000000003</v>
+        <v>37972.512000000002</v>
       </c>
       <c r="D37">
-        <v>44403.75</v>
+        <v>38987.773000000001</v>
       </c>
       <c r="E37" s="3">
-        <v>0.77453703703703702</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>112</v>
+        <v>0.77498842592592587</v>
+      </c>
+      <c r="F37" t="s">
+        <v>96</v>
       </c>
       <c r="G37" t="s">
         <v>77</v>
       </c>
       <c r="H37" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4541,25 +5502,25 @@
         <v>2023</v>
       </c>
       <c r="B38">
-        <v>37454.171999999999</v>
+        <v>39143.324000000001</v>
       </c>
       <c r="C38">
-        <v>37972.512000000002</v>
+        <v>39924.796999999999</v>
       </c>
       <c r="D38">
-        <v>38987.773000000001</v>
+        <v>41722.637000000002</v>
       </c>
       <c r="E38" s="3">
-        <v>0.77498842592592587</v>
+        <v>0.77503472222222225</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G38" t="s">
         <v>77</v>
       </c>
       <c r="H38" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -4567,50 +5528,24 @@
         <v>2023</v>
       </c>
       <c r="B39">
-        <v>39143.324000000001</v>
+        <v>36349.156000000003</v>
       </c>
       <c r="C39">
-        <v>39924.796999999999</v>
+        <v>37203.875</v>
       </c>
       <c r="D39">
-        <v>41722.637000000002</v>
+        <v>38837.214999999997</v>
       </c>
       <c r="E39" s="3">
-        <v>0.77503472222222225</v>
+        <v>0.77505787037037033</v>
       </c>
       <c r="F39" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G39" t="s">
         <v>77</v>
       </c>
       <c r="H39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2023</v>
-      </c>
-      <c r="B40">
-        <v>36349.156000000003</v>
-      </c>
-      <c r="C40">
-        <v>37203.875</v>
-      </c>
-      <c r="D40">
-        <v>38837.214999999997</v>
-      </c>
-      <c r="E40" s="3">
-        <v>0.77505787037037033</v>
-      </c>
-      <c r="F40" t="s">
-        <v>103</v>
-      </c>
-      <c r="G40" t="s">
-        <v>77</v>
-      </c>
-      <c r="H40" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>